<commit_message>
entradas excel hasta 8
</commit_message>
<xml_diff>
--- a/GDC_01.01_input.xlsx
+++ b/GDC_01.01_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verti\Desktop\misilnl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E4CCAB-44B8-40BF-A527-0CFE0F235369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FC938F-7A17-4731-8AE1-F298B18CD57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5172" yWindow="3252" windowWidth="17280" windowHeight="8964" xr2:uid="{24CFE6BC-2681-4150-9049-8A8B5AA2A626}"/>
+    <workbookView xWindow="348" yWindow="2124" windowWidth="17280" windowHeight="8964" xr2:uid="{24CFE6BC-2681-4150-9049-8A8B5AA2A626}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DE1D04-1E18-49E4-A463-124A0BC9E43B}">
   <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65:C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,7 +533,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D5">
         <v>190</v>
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D6">
         <v>190</v>
@@ -573,7 +573,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D7">
         <v>190</v>
@@ -593,7 +593,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D8">
         <v>190</v>
@@ -613,7 +613,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D9">
         <v>190</v>
@@ -633,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D10">
         <v>190</v>
@@ -653,7 +653,7 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D11">
         <v>190</v>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D12">
         <v>190</v>
@@ -693,7 +693,7 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D13">
         <v>190</v>
@@ -713,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D14">
         <v>190</v>
@@ -733,16 +733,16 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E15">
         <v>150</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -753,10 +753,10 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E16">
         <v>150</v>
@@ -773,10 +773,10 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E17">
         <v>150</v>
@@ -793,10 +793,10 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E18">
         <v>150</v>
@@ -813,10 +813,10 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E19">
         <v>150</v>
@@ -833,10 +833,10 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E20">
         <v>150</v>
@@ -853,10 +853,10 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E21">
         <v>150</v>
@@ -873,10 +873,10 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E22">
         <v>150</v>
@@ -893,10 +893,10 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E23">
         <v>150</v>
@@ -913,10 +913,10 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E24">
         <v>150</v>
@@ -933,7 +933,7 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <v>190</v>
@@ -950,10 +950,10 @@
         <v>2.1</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D26">
         <v>190</v>
@@ -970,10 +970,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D27">
         <v>190</v>
@@ -990,10 +990,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D28">
         <v>190</v>
@@ -1010,10 +1010,10 @@
         <v>2.4</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D29">
         <v>190</v>
@@ -1030,10 +1030,10 @@
         <v>2.5</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D30">
         <v>190</v>
@@ -1050,10 +1050,10 @@
         <v>2.6</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D31">
         <v>190</v>
@@ -1070,10 +1070,10 @@
         <v>2.7</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D32">
         <v>190</v>
@@ -1090,10 +1090,10 @@
         <v>2.8</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D33">
         <v>190</v>
@@ -1110,13 +1110,13 @@
         <v>2.9</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D34">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E34">
         <v>150</v>
@@ -1130,13 +1130,13 @@
         <v>3</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D35">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E35">
         <v>150</v>
@@ -1150,13 +1150,13 @@
         <v>3.1</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D36">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E36">
         <v>150</v>
@@ -1170,13 +1170,13 @@
         <v>3.2</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D37">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E37">
         <v>150</v>
@@ -1190,13 +1190,13 @@
         <v>3.3</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D38">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E38">
         <v>150</v>
@@ -1210,13 +1210,13 @@
         <v>3.4</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D39">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E39">
         <v>150</v>
@@ -1230,13 +1230,13 @@
         <v>3.5</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D40">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E40">
         <v>150</v>
@@ -1250,13 +1250,13 @@
         <v>3.6</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D41">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E41">
         <v>150</v>
@@ -1270,13 +1270,13 @@
         <v>3.7</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D42">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E42">
         <v>150</v>
@@ -1290,13 +1290,13 @@
         <v>3.8</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D43">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E43">
         <v>150</v>
@@ -1310,13 +1310,13 @@
         <v>3.9</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D44">
-        <v>190</v>
+        <v>-15</v>
       </c>
       <c r="E44">
         <v>150</v>
@@ -1333,7 +1333,7 @@
         <v>1</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D45">
         <v>190</v>
@@ -1353,13 +1353,13 @@
         <v>1</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D46">
-        <v>190</v>
+        <v>5000</v>
       </c>
       <c r="E46">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -1373,13 +1373,13 @@
         <v>1</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D47">
-        <v>190</v>
+        <v>5000</v>
       </c>
       <c r="E47">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -1393,13 +1393,13 @@
         <v>1</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D48">
-        <v>190</v>
+        <v>5000</v>
       </c>
       <c r="E48">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -1413,13 +1413,13 @@
         <v>1</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D49">
-        <v>190</v>
+        <v>5000</v>
       </c>
       <c r="E49">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -1433,13 +1433,13 @@
         <v>1</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D50">
-        <v>190</v>
+        <v>5000</v>
       </c>
       <c r="E50">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -1453,13 +1453,13 @@
         <v>1</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D51">
-        <v>190</v>
+        <v>5000</v>
       </c>
       <c r="E51">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -1473,13 +1473,13 @@
         <v>1</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D52">
-        <v>190</v>
+        <v>5000</v>
       </c>
       <c r="E52">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -1493,13 +1493,13 @@
         <v>1</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D53">
-        <v>190</v>
+        <v>5000</v>
       </c>
       <c r="E53">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -1513,13 +1513,13 @@
         <v>1</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D54">
-        <v>190</v>
+        <v>5000</v>
       </c>
       <c r="E54">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -1542,7 +1542,7 @@
         <v>150</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1733,7 +1733,7 @@
         <v>1</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D65">
         <v>190</v>
@@ -1753,7 +1753,7 @@
         <v>1</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D66">
         <v>190</v>
@@ -1773,7 +1773,7 @@
         <v>1</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D67">
         <v>190</v>
@@ -1793,7 +1793,7 @@
         <v>1</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D68">
         <v>190</v>
@@ -1813,7 +1813,7 @@
         <v>1</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D69">
         <v>190</v>
@@ -1833,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D70">
         <v>190</v>
@@ -1853,7 +1853,7 @@
         <v>1</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D71">
         <v>190</v>
@@ -1873,7 +1873,7 @@
         <v>1</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D72">
         <v>190</v>
@@ -1893,7 +1893,7 @@
         <v>1</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D73">
         <v>190</v>
@@ -1913,7 +1913,7 @@
         <v>1</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D74">
         <v>190</v>
@@ -1933,7 +1933,7 @@
         <v>1</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D75">
         <v>190</v>
@@ -1953,7 +1953,7 @@
         <v>1</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D76">
         <v>190</v>
@@ -1973,7 +1973,7 @@
         <v>1</v>
       </c>
       <c r="C77">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D77">
         <v>190</v>

</xml_diff>